<commit_message>
maths p6 q5 and wave transmission work
</commit_message>
<xml_diff>
--- a/IB/labs/wave_transmission/E4 Wave Transmission Data.xlsx
+++ b/IB/labs/wave_transmission/E4 Wave Transmission Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IB\labs\wave_transmission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IB\labs\wave_transmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C42CCD-F552-48DE-B3AB-1A3E90F3FDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C91A1C-CF0E-43E1-AA1B-F17571237993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{2E26A866-ED06-4DC1-B845-D5346E3FE0B1}"/>
+    <workbookView xWindow="4200" yWindow="1628" windowWidth="21600" windowHeight="11332" xr2:uid="{2E26A866-ED06-4DC1-B845-D5346E3FE0B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -721,18 +721,18 @@
   <dimension ref="B2:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:G57"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -770,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2.399</v>
       </c>
@@ -792,7 +792,7 @@
         <v>300.47475000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>3</v>
       </c>
@@ -814,7 +814,7 @@
         <v>294.75</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>3.6</v>
       </c>
@@ -836,7 +836,7 @@
         <v>299.78181818181815</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -859,7 +859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -879,7 +879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>3</v>
       </c>
@@ -906,7 +906,7 @@
         <v>0.23918575063613232</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
@@ -918,7 +918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -935,7 +935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>7.4</v>
       </c>
@@ -955,7 +955,7 @@
         <v>0.56823241045662909</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -978,7 +978,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>1.4833333333333334</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>34</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1.2166666666666668</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>29</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>1.0444444444444445</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>34</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>1.1777777777777778</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>28</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>1.1583333333333332</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>29</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>1.1416666666666666</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>34</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>1.1916666666666667</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>1.3666666666666667</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>28</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>28</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>1.1583333333333332</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>29</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>29</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>1.4833333333333334</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>29</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1.0444444444444445</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>29</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>1.1416666666666666</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>34</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>1.2666666666666666</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>34</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>1.2166666666666668</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>34</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>1.1777777777777778</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>34</v>
       </c>

</xml_diff>